<commit_message>
version con ajustes en el header y borrado de clases sin uso en style scss
</commit_message>
<xml_diff>
--- a/wireframes/wireframe clinicaV3.xlsx
+++ b/wireframes/wireframe clinicaV3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoderHouse\clinicaV3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoderHouse\clinicaV3\wireframes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -47,9 +47,6 @@
     <t>div class=hero</t>
   </si>
   <si>
-    <t>div class= menu navegacion</t>
-  </si>
-  <si>
     <t>div 1</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>div class= navegadorMenu</t>
+  </si>
+  <si>
+    <t>div class= fijarMenu</t>
   </si>
 </sst>
 </file>
@@ -325,6 +325,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -334,14 +342,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,7 +625,7 @@
   <dimension ref="B1:T81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +660,7 @@
     <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
       <c r="C3" s="9" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
@@ -707,8 +707,8 @@
       <c r="B5" s="6"/>
       <c r="C5" s="10"/>
       <c r="D5" s="23"/>
-      <c r="E5" s="42" t="s">
-        <v>36</v>
+      <c r="E5" s="39" t="s">
+        <v>35</v>
       </c>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
@@ -721,7 +721,7 @@
       <c r="N5" s="34"/>
       <c r="O5" s="34"/>
       <c r="P5" s="34"/>
-      <c r="Q5" s="45"/>
+      <c r="Q5" s="42"/>
       <c r="R5" s="27"/>
       <c r="S5" s="14"/>
       <c r="T5" s="4"/>
@@ -730,23 +730,23 @@
       <c r="B6" s="6"/>
       <c r="C6" s="10"/>
       <c r="D6" s="23"/>
-      <c r="E6" s="43"/>
+      <c r="E6" s="40"/>
       <c r="F6" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
       <c r="I6" s="19"/>
-      <c r="J6" s="49"/>
+      <c r="J6" s="46"/>
       <c r="K6" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L6" s="18"/>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="19"/>
-      <c r="Q6" s="48"/>
+      <c r="Q6" s="45"/>
       <c r="R6" s="27"/>
       <c r="S6" s="14"/>
       <c r="T6" s="4"/>
@@ -755,19 +755,19 @@
       <c r="B7" s="6"/>
       <c r="C7" s="10"/>
       <c r="D7" s="23"/>
-      <c r="E7" s="43"/>
+      <c r="E7" s="40"/>
       <c r="F7" s="28"/>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
       <c r="I7" s="32"/>
-      <c r="J7" s="49"/>
+      <c r="J7" s="46"/>
       <c r="K7" s="28"/>
       <c r="L7" s="33"/>
       <c r="M7" s="33"/>
       <c r="N7" s="33"/>
       <c r="O7" s="33"/>
       <c r="P7" s="32"/>
-      <c r="Q7" s="48"/>
+      <c r="Q7" s="45"/>
       <c r="R7" s="27"/>
       <c r="S7" s="14"/>
       <c r="T7" s="4"/>
@@ -776,19 +776,19 @@
       <c r="B8" s="6"/>
       <c r="C8" s="10"/>
       <c r="D8" s="23"/>
-      <c r="E8" s="43"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="28"/>
       <c r="G8" s="33"/>
       <c r="H8" s="33"/>
       <c r="I8" s="32"/>
-      <c r="J8" s="49"/>
+      <c r="J8" s="46"/>
       <c r="K8" s="28"/>
       <c r="L8" s="33"/>
       <c r="M8" s="33"/>
       <c r="N8" s="33"/>
       <c r="O8" s="33"/>
       <c r="P8" s="32"/>
-      <c r="Q8" s="48"/>
+      <c r="Q8" s="45"/>
       <c r="R8" s="27"/>
       <c r="S8" s="14"/>
       <c r="T8" s="4"/>
@@ -797,19 +797,19 @@
       <c r="B9" s="6"/>
       <c r="C9" s="10"/>
       <c r="D9" s="23"/>
-      <c r="E9" s="43"/>
+      <c r="E9" s="40"/>
       <c r="F9" s="28"/>
       <c r="G9" s="33"/>
       <c r="H9" s="33"/>
       <c r="I9" s="32"/>
-      <c r="J9" s="49"/>
+      <c r="J9" s="46"/>
       <c r="K9" s="28"/>
       <c r="L9" s="33"/>
       <c r="M9" s="33"/>
       <c r="N9" s="33"/>
       <c r="O9" s="33"/>
       <c r="P9" s="32"/>
-      <c r="Q9" s="48"/>
+      <c r="Q9" s="45"/>
       <c r="R9" s="27"/>
       <c r="S9" s="14"/>
       <c r="T9" s="4"/>
@@ -818,19 +818,19 @@
       <c r="B10" s="6"/>
       <c r="C10" s="10"/>
       <c r="D10" s="23"/>
-      <c r="E10" s="43"/>
+      <c r="E10" s="40"/>
       <c r="F10" s="28"/>
       <c r="G10" s="33"/>
       <c r="H10" s="33"/>
       <c r="I10" s="32"/>
-      <c r="J10" s="49"/>
+      <c r="J10" s="46"/>
       <c r="K10" s="28"/>
       <c r="L10" s="33"/>
       <c r="M10" s="33"/>
       <c r="N10" s="33"/>
       <c r="O10" s="33"/>
       <c r="P10" s="32"/>
-      <c r="Q10" s="48"/>
+      <c r="Q10" s="45"/>
       <c r="R10" s="27"/>
       <c r="S10" s="14"/>
       <c r="T10" s="4"/>
@@ -839,19 +839,19 @@
       <c r="B11" s="6"/>
       <c r="C11" s="10"/>
       <c r="D11" s="23"/>
-      <c r="E11" s="43"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="28"/>
       <c r="G11" s="33"/>
       <c r="H11" s="33"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="49"/>
+      <c r="J11" s="46"/>
       <c r="K11" s="28"/>
       <c r="L11" s="33"/>
       <c r="M11" s="33"/>
       <c r="N11" s="33"/>
       <c r="O11" s="33"/>
       <c r="P11" s="32"/>
-      <c r="Q11" s="48"/>
+      <c r="Q11" s="45"/>
       <c r="R11" s="27"/>
       <c r="S11" s="14"/>
       <c r="T11" s="4"/>
@@ -860,19 +860,19 @@
       <c r="B12" s="6"/>
       <c r="C12" s="10"/>
       <c r="D12" s="23"/>
-      <c r="E12" s="43"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="29"/>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
       <c r="I12" s="31"/>
-      <c r="J12" s="49"/>
+      <c r="J12" s="46"/>
       <c r="K12" s="29"/>
       <c r="L12" s="30"/>
       <c r="M12" s="30"/>
       <c r="N12" s="30"/>
       <c r="O12" s="30"/>
       <c r="P12" s="31"/>
-      <c r="Q12" s="48"/>
+      <c r="Q12" s="45"/>
       <c r="R12" s="27"/>
       <c r="S12" s="14"/>
       <c r="T12" s="4"/>
@@ -881,19 +881,19 @@
       <c r="B13" s="6"/>
       <c r="C13" s="10"/>
       <c r="D13" s="23"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="46"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="47"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="44"/>
       <c r="R13" s="27"/>
       <c r="S13" s="14"/>
       <c r="T13" s="4"/>
@@ -1011,7 +1011,7 @@
       <c r="B19" s="6"/>
       <c r="C19" s="10"/>
       <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
+      <c r="E19" s="27"/>
       <c r="F19" s="17"/>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
@@ -1023,7 +1023,7 @@
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
       <c r="P19" s="19"/>
-      <c r="Q19" s="32"/>
+      <c r="Q19" s="23"/>
       <c r="R19" s="27"/>
       <c r="S19" s="14"/>
       <c r="T19" s="4"/>
@@ -1032,7 +1032,7 @@
       <c r="B20" s="6"/>
       <c r="C20" s="10"/>
       <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
+      <c r="E20" s="27"/>
       <c r="F20" s="28"/>
       <c r="G20" s="33" t="s">
         <v>4</v>
@@ -1046,7 +1046,7 @@
       <c r="N20" s="33"/>
       <c r="O20" s="33"/>
       <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
+      <c r="Q20" s="23"/>
       <c r="R20" s="27"/>
       <c r="S20" s="14"/>
       <c r="T20" s="4"/>
@@ -1055,7 +1055,7 @@
       <c r="B21" s="6"/>
       <c r="C21" s="10"/>
       <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
+      <c r="E21" s="27"/>
       <c r="F21" s="29"/>
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
@@ -1067,7 +1067,7 @@
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
       <c r="P21" s="31"/>
-      <c r="Q21" s="32"/>
+      <c r="Q21" s="23"/>
       <c r="R21" s="27"/>
       <c r="S21" s="14"/>
       <c r="T21" s="4"/>
@@ -1162,7 +1162,7 @@
     <row r="27" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6"/>
       <c r="C27" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
@@ -1186,7 +1186,7 @@
       <c r="B28" s="6"/>
       <c r="C28" s="10"/>
       <c r="D28" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
@@ -1211,19 +1211,19 @@
       <c r="D29" s="23"/>
       <c r="E29" s="23"/>
       <c r="F29" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G29" s="18"/>
       <c r="H29" s="19"/>
       <c r="I29" s="35"/>
       <c r="J29" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K29" s="18"/>
       <c r="L29" s="19"/>
       <c r="M29" s="35"/>
       <c r="N29" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O29" s="18"/>
       <c r="P29" s="19"/>
@@ -1258,23 +1258,23 @@
       <c r="C31" s="10"/>
       <c r="D31" s="23"/>
       <c r="E31" s="23"/>
-      <c r="F31" s="39" t="s">
+      <c r="F31" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="48"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="40"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="39" t="s">
+      <c r="K31" s="48"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="K31" s="40"/>
-      <c r="L31" s="41"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="O31" s="40"/>
-      <c r="P31" s="41"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="49"/>
       <c r="Q31" s="38"/>
       <c r="R31" s="27"/>
       <c r="S31" s="14"/>
@@ -1409,7 +1409,7 @@
     <row r="38" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="6"/>
       <c r="C38" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
@@ -1458,7 +1458,7 @@
       <c r="D40" s="23"/>
       <c r="E40" s="23"/>
       <c r="F40" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
@@ -1466,7 +1466,7 @@
       <c r="J40" s="19"/>
       <c r="K40" s="35"/>
       <c r="L40" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M40" s="18"/>
       <c r="N40" s="18"/>
@@ -1504,19 +1504,19 @@
       <c r="D42" s="23"/>
       <c r="E42" s="23"/>
       <c r="F42" s="28"/>
-      <c r="G42" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
+      <c r="G42" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="48"/>
+      <c r="I42" s="48"/>
       <c r="J42" s="32"/>
       <c r="K42" s="35"/>
       <c r="L42" s="28"/>
-      <c r="M42" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="N42" s="40"/>
-      <c r="O42" s="40"/>
+      <c r="M42" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="N42" s="48"/>
+      <c r="O42" s="48"/>
       <c r="P42" s="32"/>
       <c r="Q42" s="32"/>
       <c r="R42" s="27"/>
@@ -1535,11 +1535,11 @@
       <c r="J43" s="32"/>
       <c r="K43" s="35"/>
       <c r="L43" s="28"/>
-      <c r="M43" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="N43" s="40"/>
-      <c r="O43" s="40"/>
+      <c r="M43" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="N43" s="48"/>
+      <c r="O43" s="48"/>
       <c r="P43" s="32"/>
       <c r="Q43" s="32"/>
       <c r="R43" s="27"/>
@@ -1654,7 +1654,7 @@
     <row r="49" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="6"/>
       <c r="C49" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
@@ -1678,7 +1678,7 @@
       <c r="B50" s="6"/>
       <c r="C50" s="10"/>
       <c r="D50" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E50" s="21"/>
       <c r="F50" s="21"/>
@@ -1703,19 +1703,19 @@
       <c r="D51" s="23"/>
       <c r="E51" s="23"/>
       <c r="F51" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G51" s="18"/>
       <c r="H51" s="19"/>
       <c r="I51" s="35"/>
       <c r="J51" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K51" s="18"/>
       <c r="L51" s="19"/>
       <c r="M51" s="35"/>
       <c r="N51" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O51" s="18"/>
       <c r="P51" s="19"/>
@@ -1750,23 +1750,23 @@
       <c r="C53" s="10"/>
       <c r="D53" s="23"/>
       <c r="E53" s="23"/>
-      <c r="F53" s="39" t="s">
+      <c r="F53" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="48"/>
+      <c r="H53" s="49"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="G53" s="40"/>
-      <c r="H53" s="41"/>
-      <c r="I53" s="35"/>
-      <c r="J53" s="39" t="s">
+      <c r="K53" s="48"/>
+      <c r="L53" s="49"/>
+      <c r="M53" s="35"/>
+      <c r="N53" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="K53" s="40"/>
-      <c r="L53" s="41"/>
-      <c r="M53" s="35"/>
-      <c r="N53" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="O53" s="40"/>
-      <c r="P53" s="41"/>
+      <c r="O53" s="48"/>
+      <c r="P53" s="49"/>
       <c r="Q53" s="38"/>
       <c r="R53" s="27"/>
       <c r="S53" s="14"/>
@@ -1901,7 +1901,7 @@
     <row r="60" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="6"/>
       <c r="C60" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="12"/>
@@ -1925,7 +1925,7 @@
       <c r="B61" s="6"/>
       <c r="C61" s="10"/>
       <c r="D61" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -1950,7 +1950,7 @@
       <c r="D62" s="23"/>
       <c r="E62" s="23"/>
       <c r="F62" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G62" s="18"/>
       <c r="H62" s="18"/>
@@ -1958,7 +1958,7 @@
       <c r="J62" s="19"/>
       <c r="K62" s="35"/>
       <c r="L62" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M62" s="18"/>
       <c r="N62" s="18"/>
@@ -1995,21 +1995,21 @@
       <c r="C64" s="10"/>
       <c r="D64" s="23"/>
       <c r="E64" s="23"/>
-      <c r="F64" s="39" t="s">
+      <c r="F64" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="G64" s="48"/>
+      <c r="H64" s="48"/>
+      <c r="I64" s="48"/>
+      <c r="J64" s="49"/>
+      <c r="K64" s="35"/>
+      <c r="L64" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="G64" s="40"/>
-      <c r="H64" s="40"/>
-      <c r="I64" s="40"/>
-      <c r="J64" s="41"/>
-      <c r="K64" s="35"/>
-      <c r="L64" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="M64" s="40"/>
-      <c r="N64" s="40"/>
-      <c r="O64" s="40"/>
-      <c r="P64" s="41"/>
+      <c r="M64" s="48"/>
+      <c r="N64" s="48"/>
+      <c r="O64" s="48"/>
+      <c r="P64" s="49"/>
       <c r="Q64" s="38"/>
       <c r="R64" s="27"/>
       <c r="S64" s="14"/>
@@ -2144,7 +2144,7 @@
     <row r="71" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -2168,7 +2168,7 @@
     <row r="73" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="6"/>
       <c r="C73" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
@@ -2192,7 +2192,7 @@
       <c r="B74" s="6"/>
       <c r="C74" s="10"/>
       <c r="D74" s="20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E74" s="21"/>
       <c r="F74" s="21"/>
@@ -2202,7 +2202,7 @@
       <c r="J74" s="22"/>
       <c r="K74" s="37"/>
       <c r="L74" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M74" s="21"/>
       <c r="N74" s="21"/>
@@ -2219,7 +2219,7 @@
       <c r="D75" s="23"/>
       <c r="E75" s="23"/>
       <c r="F75" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G75" s="18"/>
       <c r="H75" s="18"/>
@@ -2228,7 +2228,7 @@
       <c r="K75" s="37"/>
       <c r="L75" s="23"/>
       <c r="M75" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N75" s="18"/>
       <c r="O75" s="18"/>
@@ -2265,7 +2265,7 @@
       <c r="D77" s="23"/>
       <c r="E77" s="23"/>
       <c r="F77" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G77" s="33"/>
       <c r="H77" s="33"/>
@@ -2274,7 +2274,7 @@
       <c r="K77" s="37"/>
       <c r="L77" s="23"/>
       <c r="M77" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N77" s="33"/>
       <c r="O77" s="33"/>
@@ -2370,17 +2370,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="M43:O43"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="N31:P31"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="M42:O42"/>
     <mergeCell ref="F53:H53"/>
     <mergeCell ref="J53:L53"/>
     <mergeCell ref="N53:P53"/>
     <mergeCell ref="F64:J64"/>
     <mergeCell ref="L64:P64"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="N31:P31"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="M42:O42"/>
-    <mergeCell ref="M43:O43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
agregando segunda seccion de main en el index, crear archivo querys.scss s
</commit_message>
<xml_diff>
--- a/wireframes/wireframe clinicaV3.xlsx
+++ b/wireframes/wireframe clinicaV3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17145" windowHeight="5985"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17145" windowHeight="5985"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -322,9 +322,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -333,13 +330,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="S78" sqref="S78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +707,7 @@
       <c r="B5" s="6"/>
       <c r="C5" s="10"/>
       <c r="D5" s="23"/>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="38" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="34"/>
@@ -721,7 +721,7 @@
       <c r="N5" s="34"/>
       <c r="O5" s="34"/>
       <c r="P5" s="34"/>
-      <c r="Q5" s="42"/>
+      <c r="Q5" s="41"/>
       <c r="R5" s="27"/>
       <c r="S5" s="14"/>
       <c r="T5" s="4"/>
@@ -730,14 +730,14 @@
       <c r="B6" s="6"/>
       <c r="C6" s="10"/>
       <c r="D6" s="23"/>
-      <c r="E6" s="40"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="17" t="s">
         <v>34</v>
       </c>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
       <c r="I6" s="19"/>
-      <c r="J6" s="46"/>
+      <c r="J6" s="45"/>
       <c r="K6" s="17" t="s">
         <v>36</v>
       </c>
@@ -746,7 +746,7 @@
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="19"/>
-      <c r="Q6" s="45"/>
+      <c r="Q6" s="44"/>
       <c r="R6" s="27"/>
       <c r="S6" s="14"/>
       <c r="T6" s="4"/>
@@ -755,19 +755,19 @@
       <c r="B7" s="6"/>
       <c r="C7" s="10"/>
       <c r="D7" s="23"/>
-      <c r="E7" s="40"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="28"/>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
       <c r="I7" s="32"/>
-      <c r="J7" s="46"/>
+      <c r="J7" s="45"/>
       <c r="K7" s="28"/>
       <c r="L7" s="33"/>
       <c r="M7" s="33"/>
       <c r="N7" s="33"/>
       <c r="O7" s="33"/>
       <c r="P7" s="32"/>
-      <c r="Q7" s="45"/>
+      <c r="Q7" s="44"/>
       <c r="R7" s="27"/>
       <c r="S7" s="14"/>
       <c r="T7" s="4"/>
@@ -776,19 +776,19 @@
       <c r="B8" s="6"/>
       <c r="C8" s="10"/>
       <c r="D8" s="23"/>
-      <c r="E8" s="40"/>
+      <c r="E8" s="39"/>
       <c r="F8" s="28"/>
       <c r="G8" s="33"/>
       <c r="H8" s="33"/>
       <c r="I8" s="32"/>
-      <c r="J8" s="46"/>
+      <c r="J8" s="45"/>
       <c r="K8" s="28"/>
       <c r="L8" s="33"/>
       <c r="M8" s="33"/>
       <c r="N8" s="33"/>
       <c r="O8" s="33"/>
       <c r="P8" s="32"/>
-      <c r="Q8" s="45"/>
+      <c r="Q8" s="44"/>
       <c r="R8" s="27"/>
       <c r="S8" s="14"/>
       <c r="T8" s="4"/>
@@ -797,19 +797,19 @@
       <c r="B9" s="6"/>
       <c r="C9" s="10"/>
       <c r="D9" s="23"/>
-      <c r="E9" s="40"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="28"/>
       <c r="G9" s="33"/>
       <c r="H9" s="33"/>
       <c r="I9" s="32"/>
-      <c r="J9" s="46"/>
+      <c r="J9" s="45"/>
       <c r="K9" s="28"/>
       <c r="L9" s="33"/>
       <c r="M9" s="33"/>
       <c r="N9" s="33"/>
       <c r="O9" s="33"/>
       <c r="P9" s="32"/>
-      <c r="Q9" s="45"/>
+      <c r="Q9" s="44"/>
       <c r="R9" s="27"/>
       <c r="S9" s="14"/>
       <c r="T9" s="4"/>
@@ -818,19 +818,19 @@
       <c r="B10" s="6"/>
       <c r="C10" s="10"/>
       <c r="D10" s="23"/>
-      <c r="E10" s="40"/>
+      <c r="E10" s="39"/>
       <c r="F10" s="28"/>
       <c r="G10" s="33"/>
       <c r="H10" s="33"/>
       <c r="I10" s="32"/>
-      <c r="J10" s="46"/>
+      <c r="J10" s="45"/>
       <c r="K10" s="28"/>
       <c r="L10" s="33"/>
       <c r="M10" s="33"/>
       <c r="N10" s="33"/>
       <c r="O10" s="33"/>
       <c r="P10" s="32"/>
-      <c r="Q10" s="45"/>
+      <c r="Q10" s="44"/>
       <c r="R10" s="27"/>
       <c r="S10" s="14"/>
       <c r="T10" s="4"/>
@@ -839,19 +839,19 @@
       <c r="B11" s="6"/>
       <c r="C11" s="10"/>
       <c r="D11" s="23"/>
-      <c r="E11" s="40"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="28"/>
       <c r="G11" s="33"/>
       <c r="H11" s="33"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="46"/>
+      <c r="J11" s="45"/>
       <c r="K11" s="28"/>
       <c r="L11" s="33"/>
       <c r="M11" s="33"/>
       <c r="N11" s="33"/>
       <c r="O11" s="33"/>
       <c r="P11" s="32"/>
-      <c r="Q11" s="45"/>
+      <c r="Q11" s="44"/>
       <c r="R11" s="27"/>
       <c r="S11" s="14"/>
       <c r="T11" s="4"/>
@@ -860,19 +860,19 @@
       <c r="B12" s="6"/>
       <c r="C12" s="10"/>
       <c r="D12" s="23"/>
-      <c r="E12" s="40"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="29"/>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
       <c r="I12" s="31"/>
-      <c r="J12" s="46"/>
+      <c r="J12" s="45"/>
       <c r="K12" s="29"/>
       <c r="L12" s="30"/>
       <c r="M12" s="30"/>
       <c r="N12" s="30"/>
       <c r="O12" s="30"/>
       <c r="P12" s="31"/>
-      <c r="Q12" s="45"/>
+      <c r="Q12" s="44"/>
       <c r="R12" s="27"/>
       <c r="S12" s="14"/>
       <c r="T12" s="4"/>
@@ -881,19 +881,19 @@
       <c r="B13" s="6"/>
       <c r="C13" s="10"/>
       <c r="D13" s="23"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="44"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="43"/>
       <c r="R13" s="27"/>
       <c r="S13" s="14"/>
       <c r="T13" s="4"/>
@@ -1209,7 +1209,7 @@
       <c r="B29" s="6"/>
       <c r="C29" s="10"/>
       <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
+      <c r="E29" s="27"/>
       <c r="F29" s="17" t="s">
         <v>7</v>
       </c>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="O29" s="18"/>
       <c r="P29" s="19"/>
-      <c r="Q29" s="32"/>
+      <c r="Q29" s="23"/>
       <c r="R29" s="27"/>
       <c r="S29" s="14"/>
       <c r="T29" s="4"/>
@@ -1236,7 +1236,7 @@
       <c r="B30" s="6"/>
       <c r="C30" s="10"/>
       <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
+      <c r="E30" s="27"/>
       <c r="F30" s="28"/>
       <c r="G30" s="33"/>
       <c r="H30" s="32"/>
@@ -1248,7 +1248,7 @@
       <c r="N30" s="28"/>
       <c r="O30" s="33"/>
       <c r="P30" s="32"/>
-      <c r="Q30" s="32"/>
+      <c r="Q30" s="23"/>
       <c r="R30" s="27"/>
       <c r="S30" s="14"/>
       <c r="T30" s="4"/>
@@ -1257,25 +1257,25 @@
       <c r="B31" s="6"/>
       <c r="C31" s="10"/>
       <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
+      <c r="E31" s="27"/>
       <c r="F31" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="48"/>
-      <c r="H31" s="49"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="48"/>
       <c r="I31" s="35"/>
       <c r="J31" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="K31" s="48"/>
-      <c r="L31" s="49"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="48"/>
       <c r="M31" s="35"/>
       <c r="N31" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="O31" s="48"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="38"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="49"/>
       <c r="R31" s="27"/>
       <c r="S31" s="14"/>
       <c r="T31" s="4"/>
@@ -1284,7 +1284,7 @@
       <c r="B32" s="6"/>
       <c r="C32" s="10"/>
       <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
+      <c r="E32" s="27"/>
       <c r="F32" s="28"/>
       <c r="G32" s="33"/>
       <c r="H32" s="32"/>
@@ -1296,7 +1296,7 @@
       <c r="N32" s="28"/>
       <c r="O32" s="33"/>
       <c r="P32" s="32"/>
-      <c r="Q32" s="32"/>
+      <c r="Q32" s="23"/>
       <c r="R32" s="27"/>
       <c r="S32" s="14"/>
       <c r="T32" s="4"/>
@@ -1305,7 +1305,7 @@
       <c r="B33" s="6"/>
       <c r="C33" s="10"/>
       <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
+      <c r="E33" s="27"/>
       <c r="F33" s="28"/>
       <c r="G33" s="33"/>
       <c r="H33" s="32"/>
@@ -1317,7 +1317,7 @@
       <c r="N33" s="28"/>
       <c r="O33" s="33"/>
       <c r="P33" s="32"/>
-      <c r="Q33" s="32"/>
+      <c r="Q33" s="23"/>
       <c r="R33" s="27"/>
       <c r="S33" s="14"/>
       <c r="T33" s="4"/>
@@ -1326,7 +1326,7 @@
       <c r="B34" s="6"/>
       <c r="C34" s="10"/>
       <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
+      <c r="E34" s="27"/>
       <c r="F34" s="29"/>
       <c r="G34" s="30"/>
       <c r="H34" s="31"/>
@@ -1338,7 +1338,7 @@
       <c r="N34" s="29"/>
       <c r="O34" s="30"/>
       <c r="P34" s="31"/>
-      <c r="Q34" s="32"/>
+      <c r="Q34" s="23"/>
       <c r="R34" s="27"/>
       <c r="S34" s="14"/>
       <c r="T34" s="4"/>
@@ -1456,7 +1456,7 @@
       <c r="B40" s="6"/>
       <c r="C40" s="10"/>
       <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
+      <c r="E40" s="27"/>
       <c r="F40" s="17" t="s">
         <v>15</v>
       </c>
@@ -1472,7 +1472,7 @@
       <c r="N40" s="18"/>
       <c r="O40" s="18"/>
       <c r="P40" s="19"/>
-      <c r="Q40" s="32"/>
+      <c r="Q40" s="23"/>
       <c r="R40" s="27"/>
       <c r="S40" s="14"/>
       <c r="T40" s="4"/>
@@ -1481,7 +1481,7 @@
       <c r="B41" s="6"/>
       <c r="C41" s="10"/>
       <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
+      <c r="E41" s="27"/>
       <c r="F41" s="28"/>
       <c r="G41" s="33"/>
       <c r="H41" s="33"/>
@@ -1493,7 +1493,7 @@
       <c r="N41" s="33"/>
       <c r="O41" s="33"/>
       <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
+      <c r="Q41" s="23"/>
       <c r="R41" s="27"/>
       <c r="S41" s="14"/>
       <c r="T41" s="4"/>
@@ -1502,23 +1502,23 @@
       <c r="B42" s="6"/>
       <c r="C42" s="10"/>
       <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
+      <c r="E42" s="27"/>
       <c r="F42" s="28"/>
-      <c r="G42" s="48" t="s">
+      <c r="G42" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
       <c r="J42" s="32"/>
       <c r="K42" s="35"/>
       <c r="L42" s="28"/>
-      <c r="M42" s="48" t="s">
+      <c r="M42" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="N42" s="48"/>
-      <c r="O42" s="48"/>
+      <c r="N42" s="46"/>
+      <c r="O42" s="46"/>
       <c r="P42" s="32"/>
-      <c r="Q42" s="32"/>
+      <c r="Q42" s="23"/>
       <c r="R42" s="27"/>
       <c r="S42" s="14"/>
       <c r="T42" s="4"/>
@@ -1527,7 +1527,7 @@
       <c r="B43" s="6"/>
       <c r="C43" s="10"/>
       <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
+      <c r="E43" s="27"/>
       <c r="F43" s="28"/>
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
@@ -1535,13 +1535,13 @@
       <c r="J43" s="32"/>
       <c r="K43" s="35"/>
       <c r="L43" s="28"/>
-      <c r="M43" s="48" t="s">
+      <c r="M43" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="N43" s="48"/>
-      <c r="O43" s="48"/>
+      <c r="N43" s="46"/>
+      <c r="O43" s="46"/>
       <c r="P43" s="32"/>
-      <c r="Q43" s="32"/>
+      <c r="Q43" s="23"/>
       <c r="R43" s="27"/>
       <c r="S43" s="14"/>
       <c r="T43" s="4"/>
@@ -1550,7 +1550,7 @@
       <c r="B44" s="6"/>
       <c r="C44" s="10"/>
       <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
+      <c r="E44" s="27"/>
       <c r="F44" s="28"/>
       <c r="G44" s="33"/>
       <c r="H44" s="33"/>
@@ -1562,7 +1562,7 @@
       <c r="N44" s="33"/>
       <c r="O44" s="33"/>
       <c r="P44" s="32"/>
-      <c r="Q44" s="32"/>
+      <c r="Q44" s="23"/>
       <c r="R44" s="27"/>
       <c r="S44" s="14"/>
       <c r="T44" s="4"/>
@@ -1571,7 +1571,7 @@
       <c r="B45" s="6"/>
       <c r="C45" s="10"/>
       <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
+      <c r="E45" s="27"/>
       <c r="F45" s="29"/>
       <c r="G45" s="30"/>
       <c r="H45" s="30"/>
@@ -1583,7 +1583,7 @@
       <c r="N45" s="30"/>
       <c r="O45" s="30"/>
       <c r="P45" s="31"/>
-      <c r="Q45" s="32"/>
+      <c r="Q45" s="23"/>
       <c r="R45" s="27"/>
       <c r="S45" s="14"/>
       <c r="T45" s="4"/>
@@ -1701,7 +1701,7 @@
       <c r="B51" s="6"/>
       <c r="C51" s="10"/>
       <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
+      <c r="E51" s="27"/>
       <c r="F51" s="17" t="s">
         <v>7</v>
       </c>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="O51" s="18"/>
       <c r="P51" s="19"/>
-      <c r="Q51" s="32"/>
+      <c r="Q51" s="23"/>
       <c r="R51" s="27"/>
       <c r="S51" s="14"/>
       <c r="T51" s="4"/>
@@ -1728,7 +1728,7 @@
       <c r="B52" s="6"/>
       <c r="C52" s="10"/>
       <c r="D52" s="23"/>
-      <c r="E52" s="23"/>
+      <c r="E52" s="27"/>
       <c r="F52" s="28"/>
       <c r="G52" s="33"/>
       <c r="H52" s="32"/>
@@ -1740,7 +1740,7 @@
       <c r="N52" s="28"/>
       <c r="O52" s="33"/>
       <c r="P52" s="32"/>
-      <c r="Q52" s="32"/>
+      <c r="Q52" s="23"/>
       <c r="R52" s="27"/>
       <c r="S52" s="14"/>
       <c r="T52" s="4"/>
@@ -1749,25 +1749,25 @@
       <c r="B53" s="6"/>
       <c r="C53" s="10"/>
       <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
+      <c r="E53" s="27"/>
       <c r="F53" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G53" s="48"/>
-      <c r="H53" s="49"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="48"/>
       <c r="I53" s="35"/>
       <c r="J53" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="K53" s="48"/>
-      <c r="L53" s="49"/>
+      <c r="K53" s="46"/>
+      <c r="L53" s="48"/>
       <c r="M53" s="35"/>
       <c r="N53" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="O53" s="48"/>
-      <c r="P53" s="49"/>
-      <c r="Q53" s="38"/>
+      <c r="O53" s="46"/>
+      <c r="P53" s="48"/>
+      <c r="Q53" s="49"/>
       <c r="R53" s="27"/>
       <c r="S53" s="14"/>
       <c r="T53" s="4"/>
@@ -1776,7 +1776,7 @@
       <c r="B54" s="6"/>
       <c r="C54" s="10"/>
       <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
+      <c r="E54" s="27"/>
       <c r="F54" s="28"/>
       <c r="G54" s="33"/>
       <c r="H54" s="32"/>
@@ -1788,7 +1788,7 @@
       <c r="N54" s="28"/>
       <c r="O54" s="33"/>
       <c r="P54" s="32"/>
-      <c r="Q54" s="32"/>
+      <c r="Q54" s="23"/>
       <c r="R54" s="27"/>
       <c r="S54" s="14"/>
       <c r="T54" s="4"/>
@@ -1797,7 +1797,7 @@
       <c r="B55" s="6"/>
       <c r="C55" s="10"/>
       <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
+      <c r="E55" s="27"/>
       <c r="F55" s="28"/>
       <c r="G55" s="33"/>
       <c r="H55" s="32"/>
@@ -1809,7 +1809,7 @@
       <c r="N55" s="28"/>
       <c r="O55" s="33"/>
       <c r="P55" s="32"/>
-      <c r="Q55" s="32"/>
+      <c r="Q55" s="23"/>
       <c r="R55" s="27"/>
       <c r="S55" s="14"/>
       <c r="T55" s="4"/>
@@ -1818,7 +1818,7 @@
       <c r="B56" s="6"/>
       <c r="C56" s="10"/>
       <c r="D56" s="23"/>
-      <c r="E56" s="23"/>
+      <c r="E56" s="27"/>
       <c r="F56" s="29"/>
       <c r="G56" s="30"/>
       <c r="H56" s="31"/>
@@ -1830,7 +1830,7 @@
       <c r="N56" s="29"/>
       <c r="O56" s="30"/>
       <c r="P56" s="31"/>
-      <c r="Q56" s="32"/>
+      <c r="Q56" s="23"/>
       <c r="R56" s="27"/>
       <c r="S56" s="14"/>
       <c r="T56" s="4"/>
@@ -1948,7 +1948,7 @@
       <c r="B62" s="6"/>
       <c r="C62" s="10"/>
       <c r="D62" s="23"/>
-      <c r="E62" s="23"/>
+      <c r="E62" s="27"/>
       <c r="F62" s="17" t="s">
         <v>7</v>
       </c>
@@ -1964,7 +1964,7 @@
       <c r="N62" s="18"/>
       <c r="O62" s="18"/>
       <c r="P62" s="19"/>
-      <c r="Q62" s="32"/>
+      <c r="Q62" s="23"/>
       <c r="R62" s="27"/>
       <c r="S62" s="14"/>
       <c r="T62" s="4"/>
@@ -1973,7 +1973,7 @@
       <c r="B63" s="6"/>
       <c r="C63" s="10"/>
       <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
+      <c r="E63" s="27"/>
       <c r="F63" s="28"/>
       <c r="G63" s="33"/>
       <c r="H63" s="33"/>
@@ -1985,7 +1985,7 @@
       <c r="N63" s="33"/>
       <c r="O63" s="33"/>
       <c r="P63" s="32"/>
-      <c r="Q63" s="32"/>
+      <c r="Q63" s="23"/>
       <c r="R63" s="27"/>
       <c r="S63" s="14"/>
       <c r="T63" s="4"/>
@@ -1994,23 +1994,23 @@
       <c r="B64" s="6"/>
       <c r="C64" s="10"/>
       <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
+      <c r="E64" s="27"/>
       <c r="F64" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="G64" s="48"/>
-      <c r="H64" s="48"/>
-      <c r="I64" s="48"/>
-      <c r="J64" s="49"/>
+      <c r="G64" s="46"/>
+      <c r="H64" s="46"/>
+      <c r="I64" s="46"/>
+      <c r="J64" s="48"/>
       <c r="K64" s="35"/>
       <c r="L64" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="M64" s="48"/>
-      <c r="N64" s="48"/>
-      <c r="O64" s="48"/>
-      <c r="P64" s="49"/>
-      <c r="Q64" s="38"/>
+      <c r="M64" s="46"/>
+      <c r="N64" s="46"/>
+      <c r="O64" s="46"/>
+      <c r="P64" s="48"/>
+      <c r="Q64" s="49"/>
       <c r="R64" s="27"/>
       <c r="S64" s="14"/>
       <c r="T64" s="4"/>
@@ -2019,7 +2019,7 @@
       <c r="B65" s="6"/>
       <c r="C65" s="10"/>
       <c r="D65" s="23"/>
-      <c r="E65" s="23"/>
+      <c r="E65" s="27"/>
       <c r="F65" s="28"/>
       <c r="G65" s="33"/>
       <c r="H65" s="33"/>
@@ -2031,7 +2031,7 @@
       <c r="N65" s="33"/>
       <c r="O65" s="33"/>
       <c r="P65" s="32"/>
-      <c r="Q65" s="32"/>
+      <c r="Q65" s="23"/>
       <c r="R65" s="27"/>
       <c r="S65" s="14"/>
       <c r="T65" s="4"/>
@@ -2040,7 +2040,7 @@
       <c r="B66" s="6"/>
       <c r="C66" s="10"/>
       <c r="D66" s="23"/>
-      <c r="E66" s="23"/>
+      <c r="E66" s="27"/>
       <c r="F66" s="28"/>
       <c r="G66" s="33"/>
       <c r="H66" s="33"/>
@@ -2052,7 +2052,7 @@
       <c r="N66" s="33"/>
       <c r="O66" s="33"/>
       <c r="P66" s="32"/>
-      <c r="Q66" s="32"/>
+      <c r="Q66" s="23"/>
       <c r="R66" s="27"/>
       <c r="S66" s="14"/>
       <c r="T66" s="4"/>
@@ -2061,7 +2061,7 @@
       <c r="B67" s="6"/>
       <c r="C67" s="10"/>
       <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
+      <c r="E67" s="27"/>
       <c r="F67" s="29"/>
       <c r="G67" s="30"/>
       <c r="H67" s="30"/>
@@ -2073,7 +2073,7 @@
       <c r="N67" s="30"/>
       <c r="O67" s="30"/>
       <c r="P67" s="31"/>
-      <c r="Q67" s="32"/>
+      <c r="Q67" s="23"/>
       <c r="R67" s="27"/>
       <c r="S67" s="14"/>
       <c r="T67" s="4"/>
@@ -2217,7 +2217,7 @@
       <c r="B75" s="6"/>
       <c r="C75" s="10"/>
       <c r="D75" s="23"/>
-      <c r="E75" s="23"/>
+      <c r="E75" s="27"/>
       <c r="F75" s="17" t="s">
         <v>30</v>
       </c>
@@ -2233,7 +2233,7 @@
       <c r="N75" s="18"/>
       <c r="O75" s="18"/>
       <c r="P75" s="19"/>
-      <c r="Q75" s="32"/>
+      <c r="Q75" s="23"/>
       <c r="R75" s="27"/>
       <c r="S75" s="14"/>
       <c r="T75" s="4"/>
@@ -2242,7 +2242,7 @@
       <c r="B76" s="6"/>
       <c r="C76" s="10"/>
       <c r="D76" s="23"/>
-      <c r="E76" s="23"/>
+      <c r="E76" s="27"/>
       <c r="F76" s="28"/>
       <c r="G76" s="33"/>
       <c r="H76" s="33"/>
@@ -2254,7 +2254,7 @@
       <c r="N76" s="33"/>
       <c r="O76" s="33"/>
       <c r="P76" s="32"/>
-      <c r="Q76" s="32"/>
+      <c r="Q76" s="23"/>
       <c r="R76" s="27"/>
       <c r="S76" s="14"/>
       <c r="T76" s="4"/>
@@ -2263,7 +2263,7 @@
       <c r="B77" s="6"/>
       <c r="C77" s="10"/>
       <c r="D77" s="23"/>
-      <c r="E77" s="23"/>
+      <c r="E77" s="27"/>
       <c r="F77" s="28" t="s">
         <v>31</v>
       </c>
@@ -2279,7 +2279,7 @@
       <c r="N77" s="33"/>
       <c r="O77" s="33"/>
       <c r="P77" s="32"/>
-      <c r="Q77" s="32"/>
+      <c r="Q77" s="23"/>
       <c r="R77" s="27"/>
       <c r="S77" s="14"/>
       <c r="T77" s="4"/>
@@ -2288,7 +2288,7 @@
       <c r="B78" s="6"/>
       <c r="C78" s="10"/>
       <c r="D78" s="23"/>
-      <c r="E78" s="23"/>
+      <c r="E78" s="27"/>
       <c r="F78" s="29"/>
       <c r="G78" s="30"/>
       <c r="H78" s="30"/>
@@ -2300,7 +2300,7 @@
       <c r="N78" s="30"/>
       <c r="O78" s="30"/>
       <c r="P78" s="31"/>
-      <c r="Q78" s="32"/>
+      <c r="Q78" s="23"/>
       <c r="R78" s="27"/>
       <c r="S78" s="14"/>
       <c r="T78" s="4"/>
@@ -2370,17 +2370,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="J53:L53"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="F64:J64"/>
+    <mergeCell ref="L64:P64"/>
     <mergeCell ref="M43:O43"/>
     <mergeCell ref="F31:H31"/>
     <mergeCell ref="J31:L31"/>
     <mergeCell ref="N31:P31"/>
     <mergeCell ref="G42:I42"/>
     <mergeCell ref="M42:O42"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="J53:L53"/>
-    <mergeCell ref="N53:P53"/>
-    <mergeCell ref="F64:J64"/>
-    <mergeCell ref="L64:P64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>